<commit_message>
Fix SearchFlightForm functions, modify search_hotels_input_data Modify read_xlsx.py
</commit_message>
<xml_diff>
--- a/utils/search_hotels_input_data.xlsx
+++ b/utils/search_hotels_input_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\PROGRAMOWANIE\Software_Testing\Projects\phptravels-selenium-py\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C1E38F-1CB8-431D-A2F2-6246F64EAA66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6961FA2-B443-40D5-B7D2-FFFCED4766C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB633A56-7CCD-4F17-9940-F6AD51EA064E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>destination</t>
   </si>
@@ -66,18 +66,6 @@
   </si>
   <si>
     <t>03/01/20</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
 </sst>
 </file>
@@ -117,7 +105,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -435,7 +423,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,11 +462,11 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -491,11 +479,11 @@
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
+      <c r="D3" s="2">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>